<commit_message>
changement type date to instant pour extension ECLAIREReviewDate (#50)
* test change type date to instant

* MaJ mapping

---------

Co-authored-by: sdemeyANS <sylvain.demey@esante.gouv.fr> be027a16027a007ce8ff183d2a775cb102a7cf39
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-condition-details.xlsx
+++ b/ig/main/StructureDefinition-eclaire-condition-details.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-06T13:17:58+00:00</t>
+    <t>2023-08-23T14:17:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -140,6 +140,10 @@
 </t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
     <t>Extension.id</t>
   </si>
   <si>
@@ -183,10 +187,6 @@
   </si>
   <si>
     <t>Element.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>Extension.url</t>
@@ -663,7 +663,7 @@
         <v>40</v>
       </c>
       <c r="AJ1" t="s" s="2">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="AK1" t="s" s="2">
         <v>36</v>
@@ -671,10 +671,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
@@ -685,7 +685,7 @@
         <v>37</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s" s="2">
         <v>36</v>
@@ -697,13 +697,13 @@
         <v>36</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -754,13 +754,13 @@
         <v>36</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AG2" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI2" t="s" s="2">
         <v>36</v>
@@ -769,15 +769,15 @@
         <v>36</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
@@ -800,13 +800,13 @@
         <v>36</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s" s="2">
         <v>27</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -845,19 +845,19 @@
         <v>36</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AD3" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>37</v>
@@ -869,7 +869,7 @@
         <v>40</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="AK3" t="s" s="2">
         <v>36</v>
@@ -888,10 +888,10 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>36</v>
@@ -965,10 +965,10 @@
         <v>56</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI4" t="s" s="2">
         <v>36</v>
@@ -996,7 +996,7 @@
         <v>37</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>36</v>
@@ -1008,7 +1008,7 @@
         <v>36</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L5" t="s" s="2">
         <v>63</v>
@@ -1071,7 +1071,7 @@
         <v>37</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI5" t="s" s="2">
         <v>40</v>

</xml_diff>